<commit_message>
Fixed several bugs with swap function and updated spreadsheet
</commit_message>
<xml_diff>
--- a/bubblesort.xlsx
+++ b/bubblesort.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steven\InClassWork\project-3-parrsm18\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{390D11F3-E25E-4DB9-B660-15E537F95CB4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE625C09-836E-4359-BB39-438BB65BF848}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ED1DE44D-A7C5-42CB-982B-737AD8114FF0}"/>
   </bookViews>
@@ -657,7 +657,7 @@
                   <c:v>2E-3</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0</c:v>
+                  <c:v>2E-3</c:v>
                 </c:pt>
                 <c:pt idx="47">
                   <c:v>1E-3</c:v>
@@ -696,22 +696,22 @@
                   <c:v>2E-3</c:v>
                 </c:pt>
                 <c:pt idx="59">
+                  <c:v>1E-3</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>3.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="61">
                   <c:v>2E-3</c:v>
                 </c:pt>
-                <c:pt idx="60">
+                <c:pt idx="62">
                   <c:v>2E-3</c:v>
                 </c:pt>
-                <c:pt idx="61">
-                  <c:v>1E-3</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>1E-3</c:v>
-                </c:pt>
                 <c:pt idx="63">
-                  <c:v>1E-3</c:v>
+                  <c:v>2E-3</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>1E-3</c:v>
+                  <c:v>2E-3</c:v>
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>2E-3</c:v>
@@ -726,10 +726,10 @@
                   <c:v>2E-3</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>1E-3</c:v>
+                  <c:v>3.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>1E-3</c:v>
+                  <c:v>2E-3</c:v>
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>2E-3</c:v>
@@ -738,55 +738,55 @@
                   <c:v>2E-3</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>1E-3</c:v>
+                  <c:v>3.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>1E-3</c:v>
+                  <c:v>2E-3</c:v>
                 </c:pt>
                 <c:pt idx="75">
+                  <c:v>3.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="76">
                   <c:v>2E-3</c:v>
                 </c:pt>
-                <c:pt idx="76">
-                  <c:v>1E-3</c:v>
-                </c:pt>
                 <c:pt idx="77">
-                  <c:v>1E-3</c:v>
+                  <c:v>3.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="78">
                   <c:v>2E-3</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>2E-3</c:v>
+                  <c:v>3.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="80">
                   <c:v>2E-3</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>1E-3</c:v>
+                  <c:v>3.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>2E-3</c:v>
+                  <c:v>3.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>2E-3</c:v>
+                  <c:v>3.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>2E-3</c:v>
+                  <c:v>3.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>2E-3</c:v>
+                  <c:v>3.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>2E-3</c:v>
+                  <c:v>3.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="87">
                   <c:v>2E-3</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>2E-3</c:v>
+                  <c:v>3.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>1E-3</c:v>
+                  <c:v>4.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="90">
                   <c:v>2E-3</c:v>
@@ -798,25 +798,25 @@
                   <c:v>2E-3</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>2E-3</c:v>
+                  <c:v>3.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>2E-3</c:v>
+                  <c:v>3.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="95">
                   <c:v>3.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>2E-3</c:v>
+                  <c:v>3.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>2E-3</c:v>
+                  <c:v>3.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>2E-3</c:v>
+                  <c:v>3.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>2E-3</c:v>
+                  <c:v>3.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="100">
                   <c:v>3.0000000000000001E-3</c:v>
@@ -1185,7 +1185,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1E-3</c:v>
@@ -1194,289 +1194,289 @@
                   <c:v>1E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1E-3</c:v>
+                  <c:v>4.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1E-3</c:v>
+                  <c:v>3.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2E-3</c:v>
+                  <c:v>4.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2E-3</c:v>
+                  <c:v>6.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.0000000000000001E-3</c:v>
+                  <c:v>1.7999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.0000000000000001E-3</c:v>
+                  <c:v>8.9999999999999993E-3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.0000000000000001E-3</c:v>
+                  <c:v>1.9E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>8.0000000000000002E-3</c:v>
+                  <c:v>1.7999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5.0000000000000001E-3</c:v>
+                  <c:v>1.2999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>6.0000000000000001E-3</c:v>
+                  <c:v>1.4999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>7.0000000000000001E-3</c:v>
+                  <c:v>2.4E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.01</c:v>
+                  <c:v>2.1000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>8.9999999999999993E-3</c:v>
+                  <c:v>4.8000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.01</c:v>
+                  <c:v>2.1999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.01</c:v>
+                  <c:v>2.5000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.0999999999999999E-2</c:v>
+                  <c:v>2.5000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.0999999999999999E-2</c:v>
+                  <c:v>2.5999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.4999999999999999E-2</c:v>
+                  <c:v>3.1E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.02</c:v>
+                  <c:v>3.1E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.02</c:v>
+                  <c:v>3.2000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.02</c:v>
+                  <c:v>3.5999999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.3E-2</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.4E-2</c:v>
+                  <c:v>4.5999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.5000000000000001E-2</c:v>
+                  <c:v>5.1999999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.4E-2</c:v>
+                  <c:v>5.0999999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.9000000000000001E-2</c:v>
+                  <c:v>5.6000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2.9000000000000001E-2</c:v>
+                  <c:v>5.3999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3.2000000000000001E-2</c:v>
+                  <c:v>6.0999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>3.3000000000000002E-2</c:v>
+                  <c:v>7.9000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>3.5999999999999997E-2</c:v>
+                  <c:v>0.11899999999999999</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>3.6999999999999998E-2</c:v>
+                  <c:v>0.114</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>3.7999999999999999E-2</c:v>
+                  <c:v>9.7000000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.04</c:v>
+                  <c:v>8.6999999999999994E-2</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>4.4999999999999998E-2</c:v>
+                  <c:v>9.5000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>4.9000000000000002E-2</c:v>
+                  <c:v>8.5999999999999993E-2</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>5.1999999999999998E-2</c:v>
+                  <c:v>0.107</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>5.2999999999999999E-2</c:v>
+                  <c:v>9.4E-2</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>5.5E-2</c:v>
+                  <c:v>0.10299999999999999</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.06</c:v>
+                  <c:v>0.11600000000000001</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>5.8999999999999997E-2</c:v>
+                  <c:v>0.114</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>5.0999999999999997E-2</c:v>
+                  <c:v>0.11600000000000001</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>5.5E-2</c:v>
+                  <c:v>0.13600000000000001</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>6.6000000000000003E-2</c:v>
+                  <c:v>0.13500000000000001</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>5.8000000000000003E-2</c:v>
+                  <c:v>0.14199999999999999</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>6.8000000000000005E-2</c:v>
+                  <c:v>0.13200000000000001</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>7.8E-2</c:v>
+                  <c:v>0.13100000000000001</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>7.2999999999999995E-2</c:v>
+                  <c:v>0.13500000000000001</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>8.6999999999999994E-2</c:v>
+                  <c:v>0.14099999999999999</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>9.2999999999999999E-2</c:v>
+                  <c:v>0.151</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>9.7000000000000003E-2</c:v>
+                  <c:v>0.153</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>9.6000000000000002E-2</c:v>
+                  <c:v>0.157</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>9.7000000000000003E-2</c:v>
+                  <c:v>0.16600000000000001</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>8.1000000000000003E-2</c:v>
+                  <c:v>0.16700000000000001</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>9.6000000000000002E-2</c:v>
+                  <c:v>0.19</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>9.2999999999999999E-2</c:v>
+                  <c:v>0.185</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.09</c:v>
+                  <c:v>0.19</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>9.4E-2</c:v>
+                  <c:v>0.192</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.10100000000000001</c:v>
+                  <c:v>0.20100000000000001</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.10199999999999999</c:v>
+                  <c:v>0.20899999999999999</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.104</c:v>
+                  <c:v>0.214</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.105</c:v>
+                  <c:v>0.221</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.112</c:v>
+                  <c:v>0.22700000000000001</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.125</c:v>
+                  <c:v>0.24199999999999999</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.121</c:v>
+                  <c:v>0.245</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.11899999999999999</c:v>
+                  <c:v>0.254</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.13300000000000001</c:v>
+                  <c:v>0.254</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.129</c:v>
+                  <c:v>0.26500000000000001</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.129</c:v>
+                  <c:v>0.27</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.13400000000000001</c:v>
+                  <c:v>0.28100000000000003</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.14000000000000001</c:v>
+                  <c:v>0.28799999999999998</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>0.14899999999999999</c:v>
+                  <c:v>0.308</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>0.14199999999999999</c:v>
+                  <c:v>0.30299999999999999</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>0.15</c:v>
+                  <c:v>0.309</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.153</c:v>
+                  <c:v>0.31900000000000001</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.154</c:v>
+                  <c:v>0.32600000000000001</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>0.159</c:v>
+                  <c:v>0.33500000000000002</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>0.17199999999999999</c:v>
+                  <c:v>0.34399999999999997</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>0.16800000000000001</c:v>
+                  <c:v>0.35399999999999998</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>0.17599999999999999</c:v>
+                  <c:v>0.36899999999999999</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>0.17699999999999999</c:v>
+                  <c:v>0.38400000000000001</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>0.17899999999999999</c:v>
+                  <c:v>0.379</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>0.185</c:v>
+                  <c:v>0.39800000000000002</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>0.191</c:v>
+                  <c:v>0.39900000000000002</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>0.19700000000000001</c:v>
+                  <c:v>0.40300000000000002</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>0.19700000000000001</c:v>
+                  <c:v>0.41699999999999998</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>0.20399999999999999</c:v>
+                  <c:v>0.42299999999999999</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>0.224</c:v>
+                  <c:v>0.441</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>0.216</c:v>
+                  <c:v>0.44600000000000001</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>0.216</c:v>
+                  <c:v>0.45600000000000002</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>0.23799999999999999</c:v>
+                  <c:v>0.46500000000000002</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>0.224</c:v>
+                  <c:v>0.47599999999999998</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>0.22900000000000001</c:v>
+                  <c:v>0.49</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>0.23100000000000001</c:v>
+                  <c:v>0.503</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>0.23599999999999999</c:v>
+                  <c:v>0.50800000000000001</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>0.24199999999999999</c:v>
+                  <c:v>0.50800000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1726,7 +1726,7 @@
         <c:crossAx val="573898992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="1.0000000000000002E-2"/>
+        <c:majorUnit val="5.000000000000001E-2"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -2364,16 +2364,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>47624</xdr:rowOff>
+      <xdr:rowOff>9524</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2701,7 +2701,7 @@
   <dimension ref="A1:C102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="K44" sqref="K44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2762,7 +2762,7 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2795,7 +2795,7 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <v>1E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -2806,7 +2806,7 @@
         <v>1E-3</v>
       </c>
       <c r="C9">
-        <v>1E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2817,7 +2817,7 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <v>2E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2828,7 +2828,7 @@
         <v>1E-3</v>
       </c>
       <c r="C11">
-        <v>2E-3</v>
+        <v>6.0000000000000001E-3</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2839,7 +2839,7 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <v>4.0000000000000001E-3</v>
+        <v>1.7999999999999999E-2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2850,7 +2850,7 @@
         <v>1E-3</v>
       </c>
       <c r="C13">
-        <v>3.0000000000000001E-3</v>
+        <v>8.9999999999999993E-3</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2861,7 +2861,7 @@
         <v>0</v>
       </c>
       <c r="C14">
-        <v>5.0000000000000001E-3</v>
+        <v>1.9E-2</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2872,7 +2872,7 @@
         <v>1E-3</v>
       </c>
       <c r="C15">
-        <v>8.0000000000000002E-3</v>
+        <v>1.7999999999999999E-2</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2883,7 +2883,7 @@
         <v>1E-3</v>
       </c>
       <c r="C16">
-        <v>5.0000000000000001E-3</v>
+        <v>1.2999999999999999E-2</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2894,7 +2894,7 @@
         <v>0</v>
       </c>
       <c r="C17">
-        <v>6.0000000000000001E-3</v>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2905,7 +2905,7 @@
         <v>0</v>
       </c>
       <c r="C18">
-        <v>7.0000000000000001E-3</v>
+        <v>2.4E-2</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2916,7 +2916,7 @@
         <v>1E-3</v>
       </c>
       <c r="C19">
-        <v>0.01</v>
+        <v>2.1000000000000001E-2</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2927,7 +2927,7 @@
         <v>1E-3</v>
       </c>
       <c r="C20">
-        <v>8.9999999999999993E-3</v>
+        <v>4.8000000000000001E-2</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2938,7 +2938,7 @@
         <v>0</v>
       </c>
       <c r="C21">
-        <v>0.01</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2949,7 +2949,7 @@
         <v>1E-3</v>
       </c>
       <c r="C22">
-        <v>0.01</v>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -2960,7 +2960,7 @@
         <v>1E-3</v>
       </c>
       <c r="C23">
-        <v>1.0999999999999999E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -2971,7 +2971,7 @@
         <v>1E-3</v>
       </c>
       <c r="C24">
-        <v>1.0999999999999999E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -2982,7 +2982,7 @@
         <v>1E-3</v>
       </c>
       <c r="C25">
-        <v>1.4999999999999999E-2</v>
+        <v>3.1E-2</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -2993,7 +2993,7 @@
         <v>1E-3</v>
       </c>
       <c r="C26">
-        <v>0.02</v>
+        <v>3.1E-2</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -3004,7 +3004,7 @@
         <v>1E-3</v>
       </c>
       <c r="C27">
-        <v>0.02</v>
+        <v>3.2000000000000001E-2</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -3015,7 +3015,7 @@
         <v>1E-3</v>
       </c>
       <c r="C28">
-        <v>0.02</v>
+        <v>3.5999999999999997E-2</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -3026,7 +3026,7 @@
         <v>1E-3</v>
       </c>
       <c r="C29">
-        <v>2.3E-2</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -3037,7 +3037,7 @@
         <v>1E-3</v>
       </c>
       <c r="C30">
-        <v>2.4E-2</v>
+        <v>4.5999999999999999E-2</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -3048,7 +3048,7 @@
         <v>1E-3</v>
       </c>
       <c r="C31">
-        <v>2.5000000000000001E-2</v>
+        <v>5.1999999999999998E-2</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -3059,7 +3059,7 @@
         <v>1E-3</v>
       </c>
       <c r="C32">
-        <v>2.4E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -3070,7 +3070,7 @@
         <v>1E-3</v>
       </c>
       <c r="C33">
-        <v>2.9000000000000001E-2</v>
+        <v>5.6000000000000001E-2</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -3081,7 +3081,7 @@
         <v>1E-3</v>
       </c>
       <c r="C34">
-        <v>2.9000000000000001E-2</v>
+        <v>5.3999999999999999E-2</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -3092,7 +3092,7 @@
         <v>1E-3</v>
       </c>
       <c r="C35">
-        <v>3.2000000000000001E-2</v>
+        <v>6.0999999999999999E-2</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -3103,7 +3103,7 @@
         <v>1E-3</v>
       </c>
       <c r="C36">
-        <v>3.3000000000000002E-2</v>
+        <v>7.9000000000000001E-2</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -3114,7 +3114,7 @@
         <v>1E-3</v>
       </c>
       <c r="C37">
-        <v>3.5999999999999997E-2</v>
+        <v>0.11899999999999999</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -3125,7 +3125,7 @@
         <v>1E-3</v>
       </c>
       <c r="C38">
-        <v>3.6999999999999998E-2</v>
+        <v>0.114</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -3136,7 +3136,7 @@
         <v>1E-3</v>
       </c>
       <c r="C39">
-        <v>3.7999999999999999E-2</v>
+        <v>9.7000000000000003E-2</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -3147,7 +3147,7 @@
         <v>1E-3</v>
       </c>
       <c r="C40">
-        <v>0.04</v>
+        <v>8.6999999999999994E-2</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -3158,7 +3158,7 @@
         <v>1E-3</v>
       </c>
       <c r="C41">
-        <v>4.4999999999999998E-2</v>
+        <v>9.5000000000000001E-2</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -3169,7 +3169,7 @@
         <v>2E-3</v>
       </c>
       <c r="C42">
-        <v>4.9000000000000002E-2</v>
+        <v>8.5999999999999993E-2</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -3180,7 +3180,7 @@
         <v>1E-3</v>
       </c>
       <c r="C43">
-        <v>5.1999999999999998E-2</v>
+        <v>0.107</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -3191,7 +3191,7 @@
         <v>1E-3</v>
       </c>
       <c r="C44">
-        <v>5.2999999999999999E-2</v>
+        <v>9.4E-2</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -3202,7 +3202,7 @@
         <v>2E-3</v>
       </c>
       <c r="C45">
-        <v>5.5E-2</v>
+        <v>0.10299999999999999</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -3213,7 +3213,7 @@
         <v>2E-3</v>
       </c>
       <c r="C46">
-        <v>0.06</v>
+        <v>0.11600000000000001</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -3224,7 +3224,7 @@
         <v>2E-3</v>
       </c>
       <c r="C47">
-        <v>5.8999999999999997E-2</v>
+        <v>0.114</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -3232,10 +3232,10 @@
         <v>4600</v>
       </c>
       <c r="B48">
-        <v>0</v>
+        <v>2E-3</v>
       </c>
       <c r="C48">
-        <v>5.0999999999999997E-2</v>
+        <v>0.11600000000000001</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -3246,7 +3246,7 @@
         <v>1E-3</v>
       </c>
       <c r="C49">
-        <v>5.5E-2</v>
+        <v>0.13600000000000001</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -3257,7 +3257,7 @@
         <v>1E-3</v>
       </c>
       <c r="C50">
-        <v>6.6000000000000003E-2</v>
+        <v>0.13500000000000001</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -3268,7 +3268,7 @@
         <v>1E-3</v>
       </c>
       <c r="C51">
-        <v>5.8000000000000003E-2</v>
+        <v>0.14199999999999999</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -3279,7 +3279,7 @@
         <v>2E-3</v>
       </c>
       <c r="C52">
-        <v>6.8000000000000005E-2</v>
+        <v>0.13200000000000001</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -3290,7 +3290,7 @@
         <v>1E-3</v>
       </c>
       <c r="C53">
-        <v>7.8E-2</v>
+        <v>0.13100000000000001</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -3301,7 +3301,7 @@
         <v>2E-3</v>
       </c>
       <c r="C54">
-        <v>7.2999999999999995E-2</v>
+        <v>0.13500000000000001</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -3312,7 +3312,7 @@
         <v>2E-3</v>
       </c>
       <c r="C55">
-        <v>8.6999999999999994E-2</v>
+        <v>0.14099999999999999</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -3323,7 +3323,7 @@
         <v>2E-3</v>
       </c>
       <c r="C56">
-        <v>9.2999999999999999E-2</v>
+        <v>0.151</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -3334,7 +3334,7 @@
         <v>2E-3</v>
       </c>
       <c r="C57">
-        <v>9.7000000000000003E-2</v>
+        <v>0.153</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -3345,7 +3345,7 @@
         <v>2E-3</v>
       </c>
       <c r="C58">
-        <v>9.6000000000000002E-2</v>
+        <v>0.157</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -3356,7 +3356,7 @@
         <v>2E-3</v>
       </c>
       <c r="C59">
-        <v>9.7000000000000003E-2</v>
+        <v>0.16600000000000001</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -3367,7 +3367,7 @@
         <v>2E-3</v>
       </c>
       <c r="C60">
-        <v>8.1000000000000003E-2</v>
+        <v>0.16700000000000001</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -3375,10 +3375,10 @@
         <v>5900</v>
       </c>
       <c r="B61">
-        <v>2E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="C61">
-        <v>9.6000000000000002E-2</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -3386,10 +3386,10 @@
         <v>6000</v>
       </c>
       <c r="B62">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="C62">
-        <v>9.2999999999999999E-2</v>
+        <v>0.185</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -3397,10 +3397,10 @@
         <v>6100</v>
       </c>
       <c r="B63">
-        <v>1E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="C63">
-        <v>0.09</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -3408,10 +3408,10 @@
         <v>6200</v>
       </c>
       <c r="B64">
-        <v>1E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="C64">
-        <v>9.4E-2</v>
+        <v>0.192</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -3419,10 +3419,10 @@
         <v>6300</v>
       </c>
       <c r="B65">
-        <v>1E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="C65">
-        <v>0.10100000000000001</v>
+        <v>0.20100000000000001</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -3430,10 +3430,10 @@
         <v>6400</v>
       </c>
       <c r="B66">
-        <v>1E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="C66">
-        <v>0.10199999999999999</v>
+        <v>0.20899999999999999</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -3444,7 +3444,7 @@
         <v>2E-3</v>
       </c>
       <c r="C67">
-        <v>0.104</v>
+        <v>0.214</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -3455,7 +3455,7 @@
         <v>1E-3</v>
       </c>
       <c r="C68">
-        <v>0.105</v>
+        <v>0.221</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -3466,7 +3466,7 @@
         <v>2E-3</v>
       </c>
       <c r="C69">
-        <v>0.112</v>
+        <v>0.22700000000000001</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -3477,7 +3477,7 @@
         <v>2E-3</v>
       </c>
       <c r="C70">
-        <v>0.125</v>
+        <v>0.24199999999999999</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -3485,10 +3485,10 @@
         <v>6900</v>
       </c>
       <c r="B71">
-        <v>1E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="C71">
-        <v>0.121</v>
+        <v>0.245</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -3496,10 +3496,10 @@
         <v>7000</v>
       </c>
       <c r="B72">
-        <v>1E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="C72">
-        <v>0.11899999999999999</v>
+        <v>0.254</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -3510,7 +3510,7 @@
         <v>2E-3</v>
       </c>
       <c r="C73">
-        <v>0.13300000000000001</v>
+        <v>0.254</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -3521,7 +3521,7 @@
         <v>2E-3</v>
       </c>
       <c r="C74">
-        <v>0.129</v>
+        <v>0.26500000000000001</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -3529,10 +3529,10 @@
         <v>7300</v>
       </c>
       <c r="B75">
-        <v>1E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="C75">
-        <v>0.129</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -3540,10 +3540,10 @@
         <v>7400</v>
       </c>
       <c r="B76">
-        <v>1E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="C76">
-        <v>0.13400000000000001</v>
+        <v>0.28100000000000003</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -3551,10 +3551,10 @@
         <v>7500</v>
       </c>
       <c r="B77">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="C77">
-        <v>0.14000000000000001</v>
+        <v>0.28799999999999998</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -3562,10 +3562,10 @@
         <v>7600</v>
       </c>
       <c r="B78">
-        <v>1E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="C78">
-        <v>0.14899999999999999</v>
+        <v>0.308</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -3573,10 +3573,10 @@
         <v>7700</v>
       </c>
       <c r="B79">
-        <v>1E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="C79">
-        <v>0.14199999999999999</v>
+        <v>0.30299999999999999</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -3587,7 +3587,7 @@
         <v>2E-3</v>
       </c>
       <c r="C80">
-        <v>0.15</v>
+        <v>0.309</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -3595,10 +3595,10 @@
         <v>7900</v>
       </c>
       <c r="B81">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="C81">
-        <v>0.153</v>
+        <v>0.31900000000000001</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -3609,7 +3609,7 @@
         <v>2E-3</v>
       </c>
       <c r="C82">
-        <v>0.154</v>
+        <v>0.32600000000000001</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -3617,10 +3617,10 @@
         <v>8100</v>
       </c>
       <c r="B83">
-        <v>1E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="C83">
-        <v>0.159</v>
+        <v>0.33500000000000002</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -3628,10 +3628,10 @@
         <v>8200</v>
       </c>
       <c r="B84">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="C84">
-        <v>0.17199999999999999</v>
+        <v>0.34399999999999997</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -3639,10 +3639,10 @@
         <v>8300</v>
       </c>
       <c r="B85">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="C85">
-        <v>0.16800000000000001</v>
+        <v>0.35399999999999998</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -3650,10 +3650,10 @@
         <v>8400</v>
       </c>
       <c r="B86">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="C86">
-        <v>0.17599999999999999</v>
+        <v>0.36899999999999999</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -3661,10 +3661,10 @@
         <v>8500</v>
       </c>
       <c r="B87">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="C87">
-        <v>0.17699999999999999</v>
+        <v>0.38400000000000001</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -3672,10 +3672,10 @@
         <v>8600</v>
       </c>
       <c r="B88">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="C88">
-        <v>0.17899999999999999</v>
+        <v>0.379</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -3686,7 +3686,7 @@
         <v>2E-3</v>
       </c>
       <c r="C89">
-        <v>0.185</v>
+        <v>0.39800000000000002</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -3694,10 +3694,10 @@
         <v>8800</v>
       </c>
       <c r="B90">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="C90">
-        <v>0.191</v>
+        <v>0.39900000000000002</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -3705,10 +3705,10 @@
         <v>8900</v>
       </c>
       <c r="B91">
-        <v>1E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="C91">
-        <v>0.19700000000000001</v>
+        <v>0.40300000000000002</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -3719,7 +3719,7 @@
         <v>2E-3</v>
       </c>
       <c r="C92">
-        <v>0.19700000000000001</v>
+        <v>0.41699999999999998</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -3730,7 +3730,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="C93">
-        <v>0.20399999999999999</v>
+        <v>0.42299999999999999</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -3741,7 +3741,7 @@
         <v>2E-3</v>
       </c>
       <c r="C94">
-        <v>0.224</v>
+        <v>0.441</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -3749,10 +3749,10 @@
         <v>9300</v>
       </c>
       <c r="B95">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="C95">
-        <v>0.216</v>
+        <v>0.44600000000000001</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -3760,10 +3760,10 @@
         <v>9400</v>
       </c>
       <c r="B96">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="C96">
-        <v>0.216</v>
+        <v>0.45600000000000002</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -3774,7 +3774,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="C97">
-        <v>0.23799999999999999</v>
+        <v>0.46500000000000002</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -3782,10 +3782,10 @@
         <v>9600</v>
       </c>
       <c r="B98">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="C98">
-        <v>0.224</v>
+        <v>0.47599999999999998</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -3793,10 +3793,10 @@
         <v>9700</v>
       </c>
       <c r="B99">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="C99">
-        <v>0.22900000000000001</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -3804,10 +3804,10 @@
         <v>9800</v>
       </c>
       <c r="B100">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="C100">
-        <v>0.23100000000000001</v>
+        <v>0.503</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
@@ -3815,10 +3815,10 @@
         <v>9900</v>
       </c>
       <c r="B101">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="C101">
-        <v>0.23599999999999999</v>
+        <v>0.50800000000000001</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -3829,7 +3829,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="C102">
-        <v>0.24199999999999999</v>
+        <v>0.50800000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>